<commit_message>
4 tests pass.. FB GP LI Normal, ->LO button not working TW -> Technical issue GH-> not impliments the feature in the main page.
</commit_message>
<xml_diff>
--- a/resources/talentscreen-data.xlsx
+++ b/resources/talentscreen-data.xlsx
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,13 +432,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -446,10 +446,10 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -460,50 +460,50 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3" display="raj@abc.com"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3" display="raj@abc.com"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
All tests in the LoginTest Passed
</commit_message>
<xml_diff>
--- a/resources/talentscreen-data.xlsx
+++ b/resources/talentscreen-data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>USERNAME</t>
   </si>
@@ -77,7 +77,7 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>nish@nish.com</t>
+    <t>nish@n.com</t>
   </si>
 </sst>
 </file>
@@ -446,64 +446,62 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3" display="raj@abc.com"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3" display="raj@abc.com"/>
+    <hyperlink ref="A7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -603,7 +601,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,10 +643,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,19 +655,25 @@
     <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Login Tests (Postive Senarios) -> passed
</commit_message>
<xml_diff>
--- a/resources/talentscreen-data.xlsx
+++ b/resources/talentscreen-data.xlsx
@@ -409,7 +409,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,35 +476,34 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="A7" r:id="rId4" display="raj@abc.com"/>
+    <hyperlink ref="A7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>